<commit_message>
update feedback and deliverables based on updated work
</commit_message>
<xml_diff>
--- a/Petros/Deliverables Tracking.xlsx
+++ b/Petros/Deliverables Tracking.xlsx
@@ -280,8 +280,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="483">
+  <cellStyleXfs count="489">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -834,7 +840,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="483">
+  <cellStyles count="489">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1076,6 +1082,9 @@
     <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="488" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1317,6 +1326,9 @@
     <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="481" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="485" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2144,7 +2156,7 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2348,6 +2360,7 @@
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
       <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
     </row>
     <row r="9" spans="1:18" ht="16">
       <c r="A9" s="3" t="s">
@@ -2366,6 +2379,7 @@
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
       <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
     </row>
     <row r="10" spans="1:18">
       <c r="B10" s="10"/>
@@ -2383,7 +2397,8 @@
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
-      <c r="M11" s="28"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="17"/>
     </row>
     <row r="12" spans="1:18" ht="16">
       <c r="A12" s="3" t="s">
@@ -2399,6 +2414,7 @@
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
       <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="3" t="s">
@@ -2414,6 +2430,7 @@
       <c r="K13" s="25"/>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="3" t="s">
@@ -2426,6 +2443,7 @@
       <c r="K15" s="25"/>
       <c r="L15" s="25"/>
       <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="3" t="s">
@@ -2438,8 +2456,9 @@
       <c r="K16" s="25"/>
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16" s="25"/>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
@@ -2450,8 +2469,9 @@
       <c r="K17" s="25"/>
       <c r="L17" s="25"/>
       <c r="M17" s="25"/>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" s="25"/>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
         <v>46</v>
       </c>
@@ -2462,8 +2482,9 @@
       <c r="K18" s="25"/>
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18" s="25"/>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
@@ -2474,69 +2495,70 @@
       <c r="K19" s="25"/>
       <c r="L19" s="25"/>
       <c r="M19" s="25"/>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N19" s="25"/>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="11"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:14">
       <c r="A22" s="6"/>
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:14">
       <c r="A23" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:14">
       <c r="A24" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:14">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:14">
       <c r="A26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:14">
       <c r="A27" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="10"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:14">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:14">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:14">
       <c r="A30" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:14">
       <c r="A31" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B31" s="10"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:14">
       <c r="B32" s="10"/>
     </row>
   </sheetData>

</xml_diff>